<commit_message>
corrected employees 6 hours formula
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Medibiofarma/Amaia Iturmendi.xlsx
+++ b/config_files/Horarios/Medibiofarma/Amaia Iturmendi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="472">
   <si>
     <t>Calendario 2022</t>
   </si>
@@ -1435,6 +1435,12 @@
   </si>
   <si>
     <t>31/10/2022</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>0.0</t>
   </si>
 </sst>
 </file>
@@ -5751,7 +5757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="494">
+  <cellXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
@@ -6891,6 +6897,39 @@
     </xf>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="493" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -7420,36 +7459,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="true"/>
-    <col min="2" max="2" width="6.77734375" customWidth="true"/>
-    <col min="3" max="3" width="6.77734375" customWidth="true"/>
-    <col min="4" max="4" width="6.77734375" customWidth="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true"/>
-    <col min="6" max="6" width="6.77734375" customWidth="true"/>
-    <col min="7" max="7" width="6.77734375" customWidth="true"/>
-    <col min="8" max="8" width="6.77734375" customWidth="true"/>
-    <col min="9" max="9" width="2.77734375" customWidth="true"/>
-    <col min="10" max="10" width="6.77734375" customWidth="true"/>
-    <col min="11" max="11" width="6.77734375" customWidth="true"/>
-    <col min="12" max="12" width="6.77734375" customWidth="true"/>
-    <col min="13" max="13" width="6.77734375" customWidth="true"/>
-    <col min="14" max="14" width="6.77734375" customWidth="true"/>
-    <col min="15" max="15" width="6.77734375" customWidth="true"/>
-    <col min="16" max="16" width="6.77734375" customWidth="true"/>
-    <col min="17" max="17" width="2.77734375" customWidth="true"/>
-    <col min="18" max="18" width="6.77734375" customWidth="true"/>
-    <col min="19" max="19" width="6.77734375" customWidth="true"/>
-    <col min="20" max="20" width="6.77734375" customWidth="true"/>
-    <col min="21" max="21" width="6.77734375" customWidth="true"/>
-    <col min="22" max="22" width="6.77734375" customWidth="true"/>
-    <col min="23" max="23" width="6.77734375" customWidth="true"/>
-    <col min="24" max="24" width="6.77734375" customWidth="true"/>
-    <col min="25" max="25" width="10.0" customWidth="true"/>
-    <col min="26" max="26" width="5.77734375" customWidth="true"/>
-    <col min="27" max="27" width="25.0" customWidth="true"/>
-    <col min="28" max="28" width="25.0" customWidth="true"/>
-    <col min="29" max="29" width="25.0" customWidth="true"/>
-    <col min="30" max="30" width="10.0" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.8" customHeight="true">
@@ -9453,23 +9492,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -10049,23 +10088,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -10652,23 +10691,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11246,23 +11285,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11848,23 +11887,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -12043,8 +12082,12 @@
       <c r="B18" s="131" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="E18" s="132"/>
+      <c r="C18" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E18" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G18" s="129" t="n">
         <f>((E18-C18)*24)-1</f>
         <v>0.0</v>
@@ -12054,8 +12097,12 @@
       <c r="B19" s="131" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="132"/>
-      <c r="E19" s="132"/>
+      <c r="C19" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E19" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G19" s="129" t="n">
         <f>((E19-C19)*24)-1</f>
         <v>0.0</v>
@@ -12065,8 +12112,12 @@
       <c r="B20" s="131" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="132"/>
-      <c r="E20" s="132"/>
+      <c r="C20" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G20" s="129" t="n">
         <f>((E20-C20)*24)-1</f>
         <v>0.0</v>
@@ -12086,11 +12137,14 @@
       <c r="B22" s="131" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="132"/>
-      <c r="E22" s="132"/>
-      <c r="G22" s="129" t="n">
-        <f>((E22-C22)*24)-1</f>
-        <v>0.0</v>
+      <c r="C22" s="132" t="s">
+        <v>470</v>
+      </c>
+      <c r="E22" s="132" t="s">
+        <v>470</v>
+      </c>
+      <c r="G22" s="129" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
@@ -12117,30 +12171,40 @@
       <c r="B25" s="131" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="G25" s="129" t="n">
-        <f>((E25-C25)*24)-1</f>
-        <v>0.0</v>
+      <c r="C25" s="132" t="s">
+        <v>470</v>
+      </c>
+      <c r="E25" s="132" t="s">
+        <v>470</v>
+      </c>
+      <c r="G25" s="129" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
       <c r="B26" s="131" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="G26" s="129" t="n">
-        <f>((E26-C26)*24)-1</f>
-        <v>0.0</v>
+      <c r="C26" s="132" t="s">
+        <v>470</v>
+      </c>
+      <c r="E26" s="132" t="s">
+        <v>470</v>
+      </c>
+      <c r="G26" s="129" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
       <c r="B27" s="131" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="132"/>
-      <c r="E27" s="132"/>
+      <c r="C27" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E27" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G27" s="129" t="n">
         <f>((E27-C27)*24)-1</f>
         <v>0.0</v>
@@ -12150,8 +12214,12 @@
       <c r="B28" s="131" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="132"/>
-      <c r="E28" s="132"/>
+      <c r="C28" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E28" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G28" s="129" t="n">
         <f>((E28-C28)*24)-1</f>
         <v>0.0</v>
@@ -12161,8 +12229,12 @@
       <c r="B29" s="131" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="132"/>
-      <c r="E29" s="132"/>
+      <c r="C29" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E29" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G29" s="129" t="n">
         <f>((E29-C29)*24)-1</f>
         <v>0.0</v>
@@ -12192,8 +12264,12 @@
       <c r="B32" s="131" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="132"/>
-      <c r="E32" s="132"/>
+      <c r="C32" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E32" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G32" s="129" t="n">
         <f>((E32-C32)*24)-1</f>
         <v>0.0</v>
@@ -12203,8 +12279,12 @@
       <c r="B33" s="131" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="132"/>
-      <c r="E33" s="132"/>
+      <c r="C33" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E33" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G33" s="129" t="n">
         <f>((E33-C33)*24)-1</f>
         <v>0.0</v>
@@ -12214,8 +12294,12 @@
       <c r="B34" s="131" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="132"/>
-      <c r="E34" s="132"/>
+      <c r="C34" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E34" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G34" s="129" t="n">
         <f>((E34-C34)*24)-1</f>
         <v>0.0</v>
@@ -12225,8 +12309,12 @@
       <c r="B35" s="131" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="132"/>
-      <c r="E35" s="132"/>
+      <c r="C35" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E35" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G35" s="129" t="n">
         <f>((E35-C35)*24)-1</f>
         <v>0.0</v>
@@ -12236,8 +12324,12 @@
       <c r="B36" s="131" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="132"/>
-      <c r="E36" s="132"/>
+      <c r="C36" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E36" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G36" s="129" t="n">
         <f>((E36-C36)*24)-1</f>
         <v>0.0</v>
@@ -12267,8 +12359,12 @@
       <c r="B39" s="131" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="132"/>
-      <c r="E39" s="132"/>
+      <c r="C39" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E39" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G39" s="129" t="n">
         <f>((E39-C39)*24)-1</f>
         <v>0.0</v>
@@ -12278,8 +12374,12 @@
       <c r="B40" s="131" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="132"/>
-      <c r="E40" s="132"/>
+      <c r="C40" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E40" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G40" s="129" t="n">
         <f>((E40-C40)*24)-1</f>
         <v>0.0</v>
@@ -12289,8 +12389,12 @@
       <c r="B41" s="131" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="132"/>
-      <c r="E41" s="132"/>
+      <c r="C41" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E41" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G41" s="129" t="n">
         <f>((E41-C41)*24)-1</f>
         <v>0.0</v>
@@ -12300,8 +12404,12 @@
       <c r="B42" s="131" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="132"/>
-      <c r="E42" s="132"/>
+      <c r="C42" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E42" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G42" s="129" t="n">
         <f>((E42-C42)*24)-1</f>
         <v>0.0</v>
@@ -12311,8 +12419,12 @@
       <c r="B43" s="131" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="132"/>
-      <c r="E43" s="132"/>
+      <c r="C43" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E43" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G43" s="129" t="n">
         <f>((E43-C43)*24)-1</f>
         <v>0.0</v>
@@ -12342,8 +12454,12 @@
       <c r="B46" s="131" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="132"/>
-      <c r="E46" s="132"/>
+      <c r="C46" s="494" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E46" s="494" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G46" s="129" t="n">
         <f>((E46-C46)*24)-1</f>
         <v>0.0</v>
@@ -12450,6 +12566,7 @@
       <c r="H62" s="143"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -12472,23 +12589,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -12646,8 +12763,12 @@
       <c r="B16" s="165" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="166"/>
-      <c r="E16" s="166"/>
+      <c r="C16" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E16" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G16" s="163" t="n">
         <f>((E16-C16)*24)-1</f>
         <v>0.0</v>
@@ -12657,8 +12778,12 @@
       <c r="B17" s="165" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="166"/>
-      <c r="E17" s="166"/>
+      <c r="C17" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E17" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G17" s="163" t="n">
         <f>((E17-C17)*24)-1</f>
         <v>0.0</v>
@@ -12668,8 +12793,12 @@
       <c r="B18" s="165" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="166"/>
-      <c r="E18" s="166"/>
+      <c r="C18" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E18" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G18" s="163" t="n">
         <f>((E18-C18)*24)-1</f>
         <v>0.0</v>
@@ -12679,8 +12808,12 @@
       <c r="B19" s="165" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="166"/>
-      <c r="E19" s="166"/>
+      <c r="C19" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E19" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G19" s="163" t="n">
         <f>((E19-C19)*24)-1</f>
         <v>0.0</v>
@@ -12710,8 +12843,12 @@
       <c r="B22" s="165" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="166"/>
-      <c r="E22" s="166"/>
+      <c r="C22" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E22" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G22" s="163" t="n">
         <f>((E22-C22)*24)-1</f>
         <v>0.0</v>
@@ -12721,8 +12858,12 @@
       <c r="B23" s="165" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="166"/>
-      <c r="E23" s="166"/>
+      <c r="C23" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E23" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G23" s="163" t="n">
         <f>((E23-C23)*24)-1</f>
         <v>0.0</v>
@@ -12732,8 +12873,12 @@
       <c r="B24" s="165" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="166"/>
-      <c r="E24" s="166"/>
+      <c r="C24" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E24" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G24" s="163" t="n">
         <f>((E24-C24)*24)-1</f>
         <v>0.0</v>
@@ -12743,8 +12888,12 @@
       <c r="B25" s="165" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="166"/>
-      <c r="E25" s="166"/>
+      <c r="C25" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E25" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G25" s="163" t="n">
         <f>((E25-C25)*24)-1</f>
         <v>0.0</v>
@@ -12754,8 +12903,12 @@
       <c r="B26" s="165" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="166"/>
-      <c r="E26" s="166"/>
+      <c r="C26" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G26" s="163" t="n">
         <f>((E26-C26)*24)-1</f>
         <v>0.0</v>
@@ -12785,8 +12938,12 @@
       <c r="B29" s="165" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="166"/>
-      <c r="E29" s="166"/>
+      <c r="C29" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E29" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G29" s="163" t="n">
         <f>((E29-C29)*24)-1</f>
         <v>0.0</v>
@@ -12796,8 +12953,12 @@
       <c r="B30" s="165" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="166"/>
-      <c r="E30" s="166"/>
+      <c r="C30" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E30" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G30" s="163" t="n">
         <f>((E30-C30)*24)-1</f>
         <v>0.0</v>
@@ -12807,8 +12968,12 @@
       <c r="B31" s="165" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="166"/>
-      <c r="E31" s="166"/>
+      <c r="C31" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E31" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G31" s="163" t="n">
         <f>((E31-C31)*24)-1</f>
         <v>0.0</v>
@@ -12818,8 +12983,12 @@
       <c r="B32" s="165" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="166"/>
-      <c r="E32" s="166"/>
+      <c r="C32" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E32" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G32" s="163" t="n">
         <f>((E32-C32)*24)-1</f>
         <v>0.0</v>
@@ -12829,8 +12998,12 @@
       <c r="B33" s="165" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="166"/>
-      <c r="E33" s="166"/>
+      <c r="C33" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E33" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G33" s="163" t="n">
         <f>((E33-C33)*24)-1</f>
         <v>0.0</v>
@@ -12860,8 +13033,12 @@
       <c r="B36" s="165" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="166"/>
-      <c r="E36" s="166"/>
+      <c r="C36" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E36" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G36" s="163" t="n">
         <f>((E36-C36)*24)-1</f>
         <v>0.0</v>
@@ -12871,8 +13048,12 @@
       <c r="B37" s="165" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="166"/>
-      <c r="E37" s="166"/>
+      <c r="C37" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E37" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G37" s="163" t="n">
         <f>((E37-C37)*24)-1</f>
         <v>0.0</v>
@@ -12882,8 +13063,12 @@
       <c r="B38" s="165" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="166"/>
-      <c r="E38" s="166"/>
+      <c r="C38" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E38" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G38" s="163" t="n">
         <f>((E38-C38)*24)-1</f>
         <v>0.0</v>
@@ -12893,8 +13078,12 @@
       <c r="B39" s="165" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="166"/>
-      <c r="E39" s="166"/>
+      <c r="C39" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E39" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G39" s="163" t="n">
         <f>((E39-C39)*24)-1</f>
         <v>0.0</v>
@@ -12904,8 +13093,12 @@
       <c r="B40" s="165" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="166"/>
-      <c r="E40" s="166"/>
+      <c r="C40" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E40" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G40" s="163" t="n">
         <f>((E40-C40)*24)-1</f>
         <v>0.0</v>
@@ -12935,8 +13128,12 @@
       <c r="B43" s="165" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="166"/>
-      <c r="E43" s="166"/>
+      <c r="C43" s="496" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E43" s="496" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G43" s="163" t="n">
         <f>((E43-C43)*24)-1</f>
         <v>0.0</v>
@@ -13059,6 +13256,7 @@
       <c r="H62" s="177"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="B58:H62"/>
@@ -13081,23 +13279,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13255,8 +13453,12 @@
       <c r="B16" s="199" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="200"/>
-      <c r="E16" s="200"/>
+      <c r="C16" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E16" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G16" s="197" t="n">
         <f>((E16-C16)*24)-1</f>
         <v>0.0</v>
@@ -13266,8 +13468,12 @@
       <c r="B17" s="199" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="200"/>
-      <c r="E17" s="200"/>
+      <c r="C17" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E17" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G17" s="197" t="n">
         <f>((E17-C17)*24)-1</f>
         <v>0.0</v>
@@ -13277,8 +13483,12 @@
       <c r="B18" s="199" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="200"/>
-      <c r="E18" s="200"/>
+      <c r="C18" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E18" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G18" s="197" t="n">
         <f>((E18-C18)*24)-1</f>
         <v>0.0</v>
@@ -13288,8 +13498,12 @@
       <c r="B19" s="199" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="200"/>
-      <c r="E19" s="200"/>
+      <c r="C19" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E19" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G19" s="197" t="n">
         <f>((E19-C19)*24)-1</f>
         <v>0.0</v>
@@ -13319,8 +13533,12 @@
       <c r="B22" s="199" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="200"/>
-      <c r="E22" s="200"/>
+      <c r="C22" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E22" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G22" s="197" t="n">
         <f>((E22-C22)*24)-1</f>
         <v>0.0</v>
@@ -13330,8 +13548,12 @@
       <c r="B23" s="199" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="200"/>
-      <c r="E23" s="200"/>
+      <c r="C23" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E23" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G23" s="197" t="n">
         <f>((E23-C23)*24)-1</f>
         <v>0.0</v>
@@ -13341,8 +13563,12 @@
       <c r="B24" s="199" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="200"/>
-      <c r="E24" s="200"/>
+      <c r="C24" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E24" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G24" s="197" t="n">
         <f>((E24-C24)*24)-1</f>
         <v>0.0</v>
@@ -13352,8 +13578,12 @@
       <c r="B25" s="199" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="200"/>
-      <c r="E25" s="200"/>
+      <c r="C25" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E25" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G25" s="197" t="n">
         <f>((E25-C25)*24)-1</f>
         <v>0.0</v>
@@ -13363,8 +13593,12 @@
       <c r="B26" s="199" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="200"/>
-      <c r="E26" s="200"/>
+      <c r="C26" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G26" s="197" t="n">
         <f>((E26-C26)*24)-1</f>
         <v>0.0</v>
@@ -13394,8 +13628,12 @@
       <c r="B29" s="199" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="200"/>
-      <c r="E29" s="200"/>
+      <c r="C29" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E29" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G29" s="197" t="n">
         <f>((E29-C29)*24)-1</f>
         <v>0.0</v>
@@ -13405,8 +13643,12 @@
       <c r="B30" s="199" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="200"/>
-      <c r="E30" s="200"/>
+      <c r="C30" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E30" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G30" s="197" t="n">
         <f>((E30-C30)*24)-1</f>
         <v>0.0</v>
@@ -13416,8 +13658,12 @@
       <c r="B31" s="199" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="200"/>
-      <c r="E31" s="200"/>
+      <c r="C31" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E31" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G31" s="197" t="n">
         <f>((E31-C31)*24)-1</f>
         <v>0.0</v>
@@ -13427,8 +13673,12 @@
       <c r="B32" s="199" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="200"/>
-      <c r="E32" s="200"/>
+      <c r="C32" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E32" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G32" s="197" t="n">
         <f>((E32-C32)*24)-1</f>
         <v>0.0</v>
@@ -13438,8 +13688,12 @@
       <c r="B33" s="199" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="200"/>
-      <c r="E33" s="200"/>
+      <c r="C33" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E33" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G33" s="197" t="n">
         <f>((E33-C33)*24)-1</f>
         <v>0.0</v>
@@ -13469,8 +13723,12 @@
       <c r="B36" s="199" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="200"/>
-      <c r="E36" s="200"/>
+      <c r="C36" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E36" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G36" s="197" t="n">
         <f>((E36-C36)*24)-1</f>
         <v>0.0</v>
@@ -13480,8 +13738,12 @@
       <c r="B37" s="199" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="200"/>
-      <c r="E37" s="200"/>
+      <c r="C37" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E37" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G37" s="197" t="n">
         <f>((E37-C37)*24)-1</f>
         <v>0.0</v>
@@ -13491,8 +13753,12 @@
       <c r="B38" s="199" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="200"/>
-      <c r="E38" s="200"/>
+      <c r="C38" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E38" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G38" s="197" t="n">
         <f>((E38-C38)*24)-1</f>
         <v>0.0</v>
@@ -13502,8 +13768,12 @@
       <c r="B39" s="199" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="200"/>
-      <c r="E39" s="200"/>
+      <c r="C39" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E39" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G39" s="197" t="n">
         <f>((E39-C39)*24)-1</f>
         <v>0.0</v>
@@ -13513,8 +13783,12 @@
       <c r="B40" s="199" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="200"/>
-      <c r="E40" s="200"/>
+      <c r="C40" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E40" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G40" s="197" t="n">
         <f>((E40-C40)*24)-1</f>
         <v>0.0</v>
@@ -13544,8 +13818,12 @@
       <c r="B43" s="199" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="200"/>
-      <c r="E43" s="200"/>
+      <c r="C43" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E43" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G43" s="197" t="n">
         <f>((E43-C43)*24)-1</f>
         <v>0.0</v>
@@ -13555,8 +13833,12 @@
       <c r="B44" s="199" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="200"/>
-      <c r="E44" s="200"/>
+      <c r="C44" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E44" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G44" s="197" t="n">
         <f>((E44-C44)*24)-1</f>
         <v>0.0</v>
@@ -13566,8 +13848,12 @@
       <c r="B45" s="199" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="200"/>
-      <c r="E45" s="200"/>
+      <c r="C45" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E45" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G45" s="197" t="n">
         <f>((E45-C45)*24)-1</f>
         <v>0.0</v>
@@ -13577,8 +13863,12 @@
       <c r="B46" s="199" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="200"/>
-      <c r="E46" s="200"/>
+      <c r="C46" s="500" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E46" s="500" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G46" s="197" t="n">
         <f>((E46-C46)*24)-1</f>
         <v>0.0</v>
@@ -13680,6 +13970,7 @@
       <c r="H62" s="210"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -13702,23 +13993,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13876,8 +14167,12 @@
       <c r="B16" s="232" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="233"/>
-      <c r="E16" s="233"/>
+      <c r="C16" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E16" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G16" s="230" t="n">
         <f>((E16-C16)*24)-1</f>
         <v>0.0</v>
@@ -13907,8 +14202,12 @@
       <c r="B19" s="232" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="E19" s="233"/>
+      <c r="C19" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E19" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G19" s="230" t="n">
         <f>((E19-C19)*24)-1</f>
         <v>0.0</v>
@@ -13918,8 +14217,12 @@
       <c r="B20" s="232" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="233"/>
-      <c r="E20" s="233"/>
+      <c r="C20" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G20" s="230" t="n">
         <f>((E20-C20)*24)-1</f>
         <v>0.0</v>
@@ -13929,8 +14232,12 @@
       <c r="B21" s="232" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="233"/>
-      <c r="E21" s="233"/>
+      <c r="C21" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E21" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G21" s="230" t="n">
         <f>((E21-C21)*24)-1</f>
         <v>0.0</v>
@@ -13940,8 +14247,12 @@
       <c r="B22" s="232" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="233"/>
-      <c r="E22" s="233"/>
+      <c r="C22" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E22" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G22" s="230" t="n">
         <f>((E22-C22)*24)-1</f>
         <v>0.0</v>
@@ -13951,8 +14262,12 @@
       <c r="B23" s="232" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="233"/>
-      <c r="E23" s="233"/>
+      <c r="C23" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E23" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G23" s="230" t="n">
         <f>((E23-C23)*24)-1</f>
         <v>0.0</v>
@@ -13982,8 +14297,12 @@
       <c r="B26" s="232" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="233"/>
-      <c r="E26" s="233"/>
+      <c r="C26" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G26" s="230" t="n">
         <f>((E26-C26)*24)-1</f>
         <v>0.0</v>
@@ -13993,8 +14312,12 @@
       <c r="B27" s="232" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="233"/>
-      <c r="E27" s="233"/>
+      <c r="C27" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E27" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G27" s="230" t="n">
         <f>((E27-C27)*24)-1</f>
         <v>0.0</v>
@@ -14004,8 +14327,12 @@
       <c r="B28" s="232" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="233"/>
-      <c r="E28" s="233"/>
+      <c r="C28" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E28" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G28" s="230" t="n">
         <f>((E28-C28)*24)-1</f>
         <v>0.0</v>
@@ -14065,8 +14392,12 @@
       <c r="B34" s="232" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="233"/>
-      <c r="E34" s="233"/>
+      <c r="C34" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E34" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G34" s="230" t="n">
         <f>((E34-C34)*24)-1</f>
         <v>0.0</v>
@@ -14076,8 +14407,12 @@
       <c r="B35" s="232" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="233"/>
-      <c r="E35" s="233"/>
+      <c r="C35" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E35" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G35" s="230" t="n">
         <f>((E35-C35)*24)-1</f>
         <v>0.0</v>
@@ -14087,8 +14422,12 @@
       <c r="B36" s="232" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="233"/>
-      <c r="E36" s="233"/>
+      <c r="C36" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E36" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G36" s="230" t="n">
         <f>((E36-C36)*24)-1</f>
         <v>0.0</v>
@@ -14098,8 +14437,12 @@
       <c r="B37" s="232" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="233"/>
-      <c r="E37" s="233"/>
+      <c r="C37" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E37" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G37" s="230" t="n">
         <f>((E37-C37)*24)-1</f>
         <v>0.0</v>
@@ -14129,8 +14472,12 @@
       <c r="B40" s="232" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="233"/>
-      <c r="E40" s="233"/>
+      <c r="C40" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E40" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G40" s="230" t="n">
         <f>((E40-C40)*24)-1</f>
         <v>0.0</v>
@@ -14140,8 +14487,12 @@
       <c r="B41" s="232" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="233"/>
-      <c r="E41" s="233"/>
+      <c r="C41" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E41" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G41" s="230" t="n">
         <f>((E41-C41)*24)-1</f>
         <v>0.0</v>
@@ -14151,8 +14502,12 @@
       <c r="B42" s="232" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="233"/>
-      <c r="E42" s="233"/>
+      <c r="C42" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E42" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G42" s="230" t="n">
         <f>((E42-C42)*24)-1</f>
         <v>0.0</v>
@@ -14162,8 +14517,12 @@
       <c r="B43" s="232" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="233"/>
-      <c r="E43" s="233"/>
+      <c r="C43" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E43" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G43" s="230" t="n">
         <f>((E43-C43)*24)-1</f>
         <v>0.0</v>
@@ -14173,8 +14532,12 @@
       <c r="B44" s="232" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="233"/>
-      <c r="E44" s="233"/>
+      <c r="C44" s="504" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E44" s="504" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G44" s="230" t="n">
         <f>((E44-C44)*24)-1</f>
         <v>0.0</v>
@@ -14291,6 +14654,7 @@
       <c r="H62" s="243"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -14313,23 +14677,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14933,23 +15297,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -15533,23 +15897,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -16136,23 +16500,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">

</xml_diff>